<commit_message>
Add research paper presentation
</commit_message>
<xml_diff>
--- a/data/experiments/pitchmap_time_measurements.xlsx
+++ b/data/experiments/pitchmap_time_measurements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\pitchmap\data\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2BCE2A-BC10-4907-BDCE-F16E9693C5AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DABB501-059A-4D0A-A817-FEC428C16759}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{52DF9144-FF87-43A5-9473-15413FC4C685}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Plik</t>
   </si>
@@ -85,12 +85,27 @@
   </si>
   <si>
     <t>ENG_POL_01_09.mp4</t>
+  </si>
+  <si>
+    <t>Liczba klatek filmu</t>
+  </si>
+  <si>
+    <t>Czas modelowania ruchu kamery</t>
+  </si>
+  <si>
+    <t>Czas kalibracji</t>
+  </si>
+  <si>
+    <t>Czas przetwarzania sekundy materiału</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,8 +135,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,15 +452,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C070DCB-F494-483F-8283-62667ECF6DB8}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="3" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -689,7 +707,7 @@
         <v>4.4900000000000002E-2</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9:G13" si="2">C9+D9</f>
+        <f t="shared" ref="G9:G12" si="2">C9+D9</f>
         <v>50.143000000000001</v>
       </c>
       <c r="H9">
@@ -811,6 +829,305 @@
       </c>
       <c r="H13">
         <f t="shared" si="3"/>
+        <v>1.7408685383082776</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f>E13/11</f>
+        <v>1.2964363636363636</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f>C13/G13</f>
+        <v>0.60246214282485944</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>667</v>
+      </c>
+      <c r="C24" s="1">
+        <v>27.719000000000001</v>
+      </c>
+      <c r="D24" s="1">
+        <v>17.632999999999999</v>
+      </c>
+      <c r="E24" s="1">
+        <f>C24+D24</f>
+        <v>45.352000000000004</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24/B24 * 24</f>
+        <v>1.6318560719640181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>480</v>
+      </c>
+      <c r="C25" s="1">
+        <v>20.471</v>
+      </c>
+      <c r="D25" s="1">
+        <v>15.55</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" ref="E25:E34" si="5">C25+D25</f>
+        <v>36.021000000000001</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" ref="F25:F35" si="6">E25/B25 * 24</f>
+        <v>1.80105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>419</v>
+      </c>
+      <c r="C26" s="1">
+        <v>16.779</v>
+      </c>
+      <c r="D26" s="1">
+        <v>8.7910000000000004</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="5"/>
+        <v>25.57</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="6"/>
+        <v>1.4646300715990452</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>461</v>
+      </c>
+      <c r="C27" s="1">
+        <v>18.826000000000001</v>
+      </c>
+      <c r="D27" s="1">
+        <v>13.858000000000001</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="5"/>
+        <v>32.683999999999997</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="6"/>
+        <v>1.7015531453362256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>300</v>
+      </c>
+      <c r="C28" s="1">
+        <v>12.023999999999999</v>
+      </c>
+      <c r="D28" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="5"/>
+        <v>23.723999999999997</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="6"/>
+        <v>1.8979199999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>660</v>
+      </c>
+      <c r="C29" s="1">
+        <v>26.542000000000002</v>
+      </c>
+      <c r="D29" s="1">
+        <v>14.87</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="5"/>
+        <v>41.411999999999999</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="6"/>
+        <v>1.5058909090909092</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>175</v>
+      </c>
+      <c r="C30" s="1">
+        <v>7.15</v>
+      </c>
+      <c r="D30" s="1">
+        <v>8.9890000000000008</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="5"/>
+        <v>16.139000000000003</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="6"/>
+        <v>2.2133485714285719</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>728</v>
+      </c>
+      <c r="C31" s="1">
+        <v>29.099</v>
+      </c>
+      <c r="D31" s="1">
+        <v>21.044</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="5"/>
+        <v>50.143000000000001</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="6"/>
+        <v>1.6530659340659342</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>501</v>
+      </c>
+      <c r="C32" s="1">
+        <v>20.062999999999999</v>
+      </c>
+      <c r="D32" s="1">
+        <v>16.742000000000001</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="5"/>
+        <v>36.805</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="6"/>
+        <v>1.7631137724550898</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>758</v>
+      </c>
+      <c r="C33" s="1">
+        <v>40.140300000000003</v>
+      </c>
+      <c r="D33" s="1">
+        <v>18.498999999999999</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="5"/>
+        <v>58.639300000000006</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="6"/>
+        <v>1.8566532981530344</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>372</v>
+      </c>
+      <c r="C34" s="1">
+        <v>22.456099999999999</v>
+      </c>
+      <c r="D34" s="1">
+        <v>11.526899999999999</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="5"/>
+        <v>33.982999999999997</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="6"/>
+        <v>2.1924516129032257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <f>SUM(B24:B34)</f>
+        <v>5521</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" ref="C35:G35" si="7">SUM(C24:C34)</f>
+        <v>241.26939999999996</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="7"/>
+        <v>159.20290000000003</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="7"/>
+        <v>400.47230000000002</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="6"/>
         <v>1.7408685383082776</v>
       </c>
     </row>

</xml_diff>